<commit_message>
IO files as provided by CEA
</commit_message>
<xml_diff>
--- a/InputData/io-model/WMITR/Worker Marg Income Tax Rate.xlsx
+++ b/InputData/io-model/WMITR/Worker Marg Income Tax Rate.xlsx
@@ -1,27 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeng\Dropbox (Energy Innovation)\Documents\Energy Policy Simulator\Models\eps-eu\InputData\io-model\WMITR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adolg\Dropbox\Energy Innovation IO\Deliverable IO files\EU\WMITR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A7503C-6834-475B-87CF-A828D044C2B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9741069-D092-4755-BF28-9336ECABBD47}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40515" yWindow="4395" windowWidth="20625" windowHeight="14865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="19500" windowHeight="18840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="WMITR" sheetId="2" r:id="rId2"/>
+    <sheet name="Calculations" sheetId="3" r:id="rId2"/>
+    <sheet name="WMITR" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -29,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Workers</t>
   </si>
@@ -46,32 +50,47 @@
     <t>Marginal Income Tax Rate (dimensionless)</t>
   </si>
   <si>
-    <t>Trading Economics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">List of Countries by Personal Income Tax Rate </t>
-  </si>
-  <si>
-    <t>https://tradingeconomics.com/country-list/personal-income-tax-rate?continent=europe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">European Union </t>
-  </si>
-  <si>
-    <t>Accessed 20th May 2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Note that this source does not specify whether this income tax applies to the average or workers, but it is likely that it is the average. </t>
-  </si>
-  <si>
-    <t>We assume that the overall difference between the overall average and worker-only value is insignificant.</t>
+    <t>Income Tax Revenue</t>
+  </si>
+  <si>
+    <t>Average real tax rate, EU28</t>
+  </si>
+  <si>
+    <t>Ratio effective marginal tax rate: average tax rate (US)</t>
+  </si>
+  <si>
+    <t>https://www.institutmolinari.org/IMG/pdf/tax-burden-eu-2018.pdf</t>
+  </si>
+  <si>
+    <t>EPS model; US WMITR</t>
+  </si>
+  <si>
+    <t>Institu Economique Molinari</t>
+  </si>
+  <si>
+    <t>The Tax Burden of Typical Workers in the EU 28 - 2018</t>
+  </si>
+  <si>
+    <t>EU average real tax rates, 2010-2016, combined average</t>
+  </si>
+  <si>
+    <t>Estimated effective marginal tax rate, EU28</t>
+  </si>
+  <si>
+    <t>(including social security contributions and VAT as well as income tax) by the US ratio</t>
+  </si>
+  <si>
+    <t>of marginal income tax rate: average income tax rate.</t>
+  </si>
+  <si>
+    <t>In the absence of data about worker marginal income tax rate, we scale the average tax rate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,16 +114,330 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Cambria"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -112,12 +445,164 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -127,10 +612,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="47">
+    <cellStyle name="20% - Accent1" xfId="23" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="27" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="31" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="35" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="39" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="43" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="24" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="28" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="32" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="36" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="40" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="44" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="25" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="29" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="33" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="37" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="41" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="45" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="22" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="26" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="30" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="34" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="38" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="42" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="11" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="15" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="17" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="20" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="10" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="6" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="7" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="8" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="9" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Input" xfId="13" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="16" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="12" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 4" xfId="46" xr:uid="{B68D24ED-2898-4F08-A697-BFF405082D30}"/>
+    <cellStyle name="Note" xfId="19" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="14" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
+    <cellStyle name="Title" xfId="5" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="21" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="18" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -466,103 +1002,173 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B12"/>
+  <sheetPr>
+    <tabColor theme="6" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B4" s="2">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B6" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B7" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>11</v>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr>
+    <tabColor theme="6" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A2:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="50.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="10">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="6">
+        <f>30/24</f>
+        <v>1.25</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="7">
+        <f>B2*B3</f>
+        <v>0.55625000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.265625" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>0.38600000000000001</v>
+      <c r="B2" s="8">
+        <f>Calculations!B4</f>
+        <v>0.55625000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>